<commit_message>
added more graphs and data for hvl at various kvp
</commit_message>
<xml_diff>
--- a/Risultati_Esperimenti.xlsx
+++ b/Risultati_Esperimenti.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="RX" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
   <si>
     <t>dose vs amps</t>
   </si>
@@ -75,6 +75,27 @@
   </si>
   <si>
     <t xml:space="preserve"> hvl 100 open</t>
+  </si>
+  <si>
+    <t>hvl 80 closed</t>
+  </si>
+  <si>
+    <t>hvl 60 closed</t>
+  </si>
+  <si>
+    <t>hvl 80 open</t>
+  </si>
+  <si>
+    <t>hvl 60 open</t>
+  </si>
+  <si>
+    <t>lineare</t>
+  </si>
+  <si>
+    <t>quadrativo</t>
+  </si>
+  <si>
+    <t>quadratico</t>
   </si>
 </sst>
 </file>
@@ -424,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -491,6 +512,9 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
       <c r="B6">
         <v>0.999</v>
       </c>
@@ -505,6 +529,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
       <c r="B7">
         <v>0.998</v>
       </c>
@@ -524,6 +551,9 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
       <c r="B9">
         <v>0.997</v>
       </c>
@@ -538,6 +568,9 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
       <c r="B10">
         <v>1</v>
       </c>
@@ -714,6 +747,258 @@
       </c>
       <c r="H24">
         <v>0.998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="D26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26">
+        <v>-6.9000000000000006E-2</v>
+      </c>
+      <c r="H26">
+        <v>0.81100000000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C28">
+        <v>0.999</v>
+      </c>
+      <c r="D28" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28">
+        <v>-1E-3</v>
+      </c>
+      <c r="F28">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G28">
+        <v>-0.22700000000000001</v>
+      </c>
+      <c r="H28">
+        <v>0.98899999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1E-4</v>
+      </c>
+      <c r="E29">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="F29">
+        <v>0.04</v>
+      </c>
+      <c r="G29">
+        <v>-0.25800000000000001</v>
+      </c>
+      <c r="H29">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="D31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31">
+        <v>-7.1999999999999995E-2</v>
+      </c>
+      <c r="H31">
+        <v>0.76300000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C33">
+        <v>0.997</v>
+      </c>
+      <c r="D33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33">
+        <v>-1E-3</v>
+      </c>
+      <c r="F33">
+        <v>-3.1E-2</v>
+      </c>
+      <c r="G33">
+        <v>-0.26700000000000002</v>
+      </c>
+      <c r="H33">
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="E34">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="F34">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="G34">
+        <v>-0.31900000000000001</v>
+      </c>
+      <c r="H34">
+        <v>0.997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="D36" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" t="s">
+        <v>4</v>
+      </c>
+      <c r="G36">
+        <v>-0.157</v>
+      </c>
+      <c r="H36">
+        <v>0.93799999999999994</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C38">
+        <v>0.997</v>
+      </c>
+      <c r="D38" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38">
+        <v>-1E-3</v>
+      </c>
+      <c r="F38">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="G38">
+        <v>-0.23799999999999999</v>
+      </c>
+      <c r="H38">
+        <v>0.98599999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1E-4</v>
+      </c>
+      <c r="E39">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="F39">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G39">
+        <v>-0.27400000000000002</v>
+      </c>
+      <c r="H39">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="D41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" t="s">
+        <v>4</v>
+      </c>
+      <c r="G41">
+        <v>-7.1999999999999995E-2</v>
+      </c>
+      <c r="H41">
+        <v>0.76200000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C43">
+        <v>0.996</v>
+      </c>
+      <c r="D43" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43">
+        <v>-1E-3</v>
+      </c>
+      <c r="F43">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="G43">
+        <v>-0.26800000000000002</v>
+      </c>
+      <c r="H43">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="E44">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="F44">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="G44">
+        <v>-0.32200000000000001</v>
+      </c>
+      <c r="H44">
+        <v>0.995</v>
       </c>
     </row>
   </sheetData>
@@ -726,7 +1011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>

</xml_diff>